<commit_message>
fix manual tests for Bulgaria
</commit_message>
<xml_diff>
--- a/manual/2020-12-22-tests-manual.xlsx
+++ b/manual/2020-12-22-tests-manual.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">country</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bulgaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 105 928</t>
   </si>
   <si>
     <t xml:space="preserve">manual</t>
@@ -156,7 +153,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -185,8 +182,8 @@
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
+      <c r="B2" s="1" t="n">
+        <v>1105928</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>4304</v>
@@ -195,7 +192,7 @@
         <v>44187</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>